<commit_message>
add graphs: bar graph, line graph & pie chart
</commit_message>
<xml_diff>
--- a/data/business_dataset.xlsx
+++ b/data/business_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amos Mungai\Desktop\university\amos\projects\data analytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953D5C6F-ACE7-47D8-87AF-0FBBC7B9F2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E997C33B-C817-415D-B3EB-EBE0A4DC6BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="686" yWindow="686" windowWidth="9814" windowHeight="8108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1970,13 +1970,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="1" width="34.3828125" customWidth="1"/>
     <col min="3" max="3" width="28.3046875" customWidth="1"/>
+    <col min="4" max="4" width="19.4609375" customWidth="1"/>
+    <col min="5" max="5" width="17.3046875" customWidth="1"/>
+    <col min="6" max="6" width="17.921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">

</xml_diff>